<commit_message>
Restore value lists sheet to test XLSXs
</commit_message>
<xml_diff>
--- a/openn/tests/data/sheets/invalid_missing_required.xlsx
+++ b/openn/tests/data/sheets/invalid_missing_required.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="6" r:id="rId1"/>
+    <sheet name="VALUE LISTS" sheetId="7" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="107">
   <si>
     <t>Note: Please enter one work per page.</t>
   </si>
@@ -307,13 +308,46 @@
   </si>
   <si>
     <t>Bound dimensions</t>
+  </si>
+  <si>
+    <t>TOC_TYPES</t>
+  </si>
+  <si>
+    <t>LICENSES</t>
+  </si>
+  <si>
+    <t>Page enumeration</t>
+  </si>
+  <si>
+    <t>TOC1</t>
+  </si>
+  <si>
+    <t>Foliation</t>
+  </si>
+  <si>
+    <t>TOC2</t>
+  </si>
+  <si>
+    <t>CC0</t>
+  </si>
+  <si>
+    <t>Pagination</t>
+  </si>
+  <si>
+    <t>TOC3</t>
+  </si>
+  <si>
+    <t>ILL</t>
+  </si>
+  <si>
+    <t>BLANK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,6 +407,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -457,7 +499,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="15" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
@@ -476,6 +518,7 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="15" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="15" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="52">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -830,7 +873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="7" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
@@ -1910,4 +1953,75 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="2" spans="2:6">
+      <c r="B2" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Use EMPTY instead of BLANK for blank fields; BLANK is a field value one the Pages sheet.
</commit_message>
<xml_diff>
--- a/openn/tests/data/sheets/invalid_missing_required.xlsx
+++ b/openn/tests/data/sheets/invalid_missing_required.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="6" r:id="rId1"/>
@@ -873,11 +873,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="7" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="C29" sqref="C29"/>
+      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1458,9 +1458,7 @@
       <c r="B28" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="11">
-        <v>1903</v>
-      </c>
+      <c r="C28" s="11"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
@@ -1959,7 +1957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>